<commit_message>
1- Enter same name and code and get the  Exist Already Message
</commit_message>
<xml_diff>
--- a/src/test/java/Apache/Resource/YB_12_SubjectCategories.xlsx
+++ b/src/test/java/Apache/Resource/YB_12_SubjectCategories.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">ka23ds</t>
+    <t xml:space="preserve">ka23dds</t>
   </si>
   <si>
-    <t xml:space="preserve">123ds</t>
+    <t xml:space="preserve">12gfds</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
1- create a searchBtnBayatlama function 2-Edit Subject Categories
</commit_message>
<xml_diff>
--- a/src/test/java/Apache/Resource/YB_12_SubjectCategories.xlsx
+++ b/src/test/java/Apache/Resource/YB_12_SubjectCategories.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">ka23dds</t>
+    <t xml:space="preserve">ka2xxyys</t>
   </si>
   <si>
-    <t xml:space="preserve">12gfds</t>
+    <t xml:space="preserve">12g23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">karsd23fg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sas234</t>
   </si>
 </sst>
 </file>
@@ -123,15 +129,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -140,6 +150,12 @@
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>